<commit_message>
Hemos cambiado la fórmula de Ventas objetivo
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_07_15022026_deco_exterior.xlsx
+++ b/data/output/Pedido_Semana_07_15022026_deco_exterior.xlsx
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="2" t="n">
         <v>0</v>
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="6" t="n">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="6" t="n">
         <v>4.95</v>
@@ -1675,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="6" t="n">
         <v>1.15</v>
@@ -2242,7 +2242,7 @@
         <v>6</v>
       </c>
       <c r="L22" s="3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M22" s="6" t="n">
         <v>19</v>
@@ -2262,7 +2262,7 @@
         <v>24</v>
       </c>
       <c r="R22" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="2" t="n">
         <v>0</v>
@@ -2323,7 +2323,7 @@
         <v>4</v>
       </c>
       <c r="L23" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M23" s="6" t="n">
         <v>6.33</v>
@@ -2343,16 +2343,16 @@
         <v>12</v>
       </c>
       <c r="R23" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="T23" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
@@ -2505,13 +2505,13 @@
         <v>0</v>
       </c>
       <c r="R25" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="T25" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U25" s="8" t="n">
         <v>0</v>
@@ -3376,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="L36" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="6" t="n">
         <v>5.55</v>
@@ -3457,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="L37" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M37" s="6" t="n">
         <v>33.8</v>
@@ -3558,13 +3558,13 @@
         <v>0</v>
       </c>
       <c r="R38" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S38" s="2" t="n">
         <v>6</v>
       </c>
       <c r="T38" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U38" s="8" t="n">
         <v>0</v>
@@ -3639,13 +3639,13 @@
         <v>0</v>
       </c>
       <c r="R39" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S39" s="2" t="n">
         <v>9</v>
       </c>
       <c r="T39" s="3" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="U39" s="8" t="n">
         <v>0</v>
@@ -3781,7 +3781,7 @@
         <v>1</v>
       </c>
       <c r="L41" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="6" t="n">
         <v>2.9</v>
@@ -4206,13 +4206,13 @@
         <v>0</v>
       </c>
       <c r="R46" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S46" s="2" t="n">
         <v>3</v>
       </c>
       <c r="T46" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U46" s="8" t="n">
         <v>0</v>
@@ -4267,7 +4267,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="3" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M47" s="6" t="n">
         <v>2.3</v>
@@ -4287,7 +4287,7 @@
         <v>3</v>
       </c>
       <c r="R47" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S47" s="2" t="n">
         <v>0</v>
@@ -4591,7 +4591,7 @@
         <v>1</v>
       </c>
       <c r="L51" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51" s="6" t="n">
         <v>1.55</v>
@@ -4672,7 +4672,7 @@
         <v>2</v>
       </c>
       <c r="L52" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52" s="6" t="n">
         <v>55.35</v>
@@ -4692,13 +4692,13 @@
         <v>0</v>
       </c>
       <c r="R52" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S52" s="2" t="n">
         <v>8</v>
       </c>
       <c r="T52" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U52" s="8" t="n">
         <v>0</v>
@@ -4854,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="R54" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S54" s="2" t="n">
         <v>0</v>
@@ -4996,7 +4996,7 @@
         <v>1</v>
       </c>
       <c r="L56" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M56" s="6" t="n">
         <v>3.5</v>
@@ -5583,13 +5583,13 @@
         <v>0</v>
       </c>
       <c r="R63" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S63" s="2" t="n">
         <v>3</v>
       </c>
       <c r="T63" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U63" s="8" t="n">
         <v>0</v>
@@ -6015,7 +6015,7 @@
         </is>
       </c>
       <c r="C71" s="5" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72">
@@ -6135,7 +6135,7 @@
         </is>
       </c>
       <c r="C82" s="5" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
seguimos con la mejora de los errores de los mails
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_07_15022026_deco_exterior.xlsx
+++ b/data/output/Pedido_Semana_07_15022026_deco_exterior.xlsx
@@ -727,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="6" t="n">
         <v>0</v>
@@ -804,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="6" t="n">
         <v>0</v>
@@ -881,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="6" t="n">
         <v>0</v>
@@ -958,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="6" t="n">
         <v>0</v>
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="6" t="n">
         <v>0</v>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="6" t="n">
         <v>0</v>
@@ -1189,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="6" t="n">
         <v>8.300000000000001</v>
@@ -1270,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10" s="6" t="n">
         <v>8.800000000000001</v>
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="6" t="n">
         <v>4.95</v>
@@ -1432,7 +1432,7 @@
         <v>2</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12" s="6" t="n">
         <v>27</v>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="6" t="n">
         <v>2.2</v>
@@ -1594,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="6" t="n">
         <v>1.45</v>
@@ -1675,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="6" t="n">
         <v>1.15</v>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="6" t="n">
         <v>53.78</v>
@@ -1837,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="6" t="n">
         <v>20.4</v>
@@ -1918,7 +1918,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="6" t="n">
         <v>5.15</v>
@@ -1999,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="6" t="n">
         <v>3.12</v>
@@ -2080,7 +2080,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="6" t="n">
         <v>16.38</v>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="6" t="n">
         <v>10.5</v>
@@ -2242,7 +2242,7 @@
         <v>6</v>
       </c>
       <c r="L22" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M22" s="6" t="n">
         <v>19</v>
@@ -2323,7 +2323,7 @@
         <v>4</v>
       </c>
       <c r="L23" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M23" s="6" t="n">
         <v>6.33</v>
@@ -2404,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="6" t="n">
         <v>6</v>
@@ -2485,7 +2485,7 @@
         <v>1</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="6" t="n">
         <v>1.25</v>
@@ -2566,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="6" t="n">
         <v>0.65</v>
@@ -2647,7 +2647,7 @@
         <v>2</v>
       </c>
       <c r="L27" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M27" s="6" t="n">
         <v>11.8</v>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
       <c r="L28" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="6" t="n">
         <v>1.15</v>
@@ -2809,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="6" t="n">
         <v>0.68</v>
@@ -2890,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="6" t="n">
         <v>11.73</v>
@@ -2971,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="6" t="n">
         <v>2.45</v>
@@ -3052,7 +3052,7 @@
         <v>1</v>
       </c>
       <c r="L32" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" s="6" t="n">
         <v>3.25</v>
@@ -3133,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="6" t="n">
         <v>5.9</v>
@@ -3214,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="L34" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="6" t="n">
         <v>45.28</v>
@@ -3295,7 +3295,7 @@
         <v>1</v>
       </c>
       <c r="L35" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="6" t="n">
         <v>2.85</v>
@@ -3376,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="L36" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="6" t="n">
         <v>5.55</v>
@@ -3457,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="L37" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M37" s="6" t="n">
         <v>33.8</v>
@@ -3538,7 +3538,7 @@
         <v>1</v>
       </c>
       <c r="L38" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="6" t="n">
         <v>23</v>
@@ -3619,7 +3619,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="6" t="n">
         <v>24.75</v>
@@ -3700,7 +3700,7 @@
         <v>1</v>
       </c>
       <c r="L40" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="6" t="n">
         <v>118.45</v>
@@ -3781,7 +3781,7 @@
         <v>1</v>
       </c>
       <c r="L41" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" s="6" t="n">
         <v>2.9</v>
@@ -3862,7 +3862,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="6" t="n">
         <v>1.3</v>
@@ -3943,7 +3943,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43" s="6" t="n">
         <v>0.85</v>
@@ -4024,7 +4024,7 @@
         <v>1</v>
       </c>
       <c r="L44" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" s="6" t="n">
         <v>0.8</v>
@@ -4105,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M45" s="6" t="n">
         <v>7.22</v>
@@ -4186,7 +4186,7 @@
         <v>1</v>
       </c>
       <c r="L46" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M46" s="6" t="n">
         <v>1.12</v>
@@ -4267,7 +4267,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="6" t="n">
         <v>2.3</v>
@@ -4348,7 +4348,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" s="6" t="n">
         <v>21.78</v>
@@ -4429,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="L49" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49" s="6" t="n">
         <v>2.05</v>
@@ -4510,7 +4510,7 @@
         <v>1</v>
       </c>
       <c r="L50" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" s="6" t="n">
         <v>1.23</v>
@@ -4591,7 +4591,7 @@
         <v>1</v>
       </c>
       <c r="L51" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" s="6" t="n">
         <v>1.55</v>
@@ -4672,7 +4672,7 @@
         <v>2</v>
       </c>
       <c r="L52" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M52" s="6" t="n">
         <v>55.35</v>
@@ -4753,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="L53" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53" s="6" t="n">
         <v>340.95</v>
@@ -4834,7 +4834,7 @@
         <v>1</v>
       </c>
       <c r="L54" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="6" t="n">
         <v>34.38</v>
@@ -4915,7 +4915,7 @@
         <v>1</v>
       </c>
       <c r="L55" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M55" s="6" t="n">
         <v>44.35</v>
@@ -4996,7 +4996,7 @@
         <v>1</v>
       </c>
       <c r="L56" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" s="6" t="n">
         <v>3.5</v>
@@ -5077,7 +5077,7 @@
         <v>1</v>
       </c>
       <c r="L57" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M57" s="6" t="n">
         <v>2.12</v>
@@ -5158,7 +5158,7 @@
         <v>2</v>
       </c>
       <c r="L58" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M58" s="6" t="n">
         <v>12.75</v>
@@ -5239,7 +5239,7 @@
         <v>1</v>
       </c>
       <c r="L59" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" s="6" t="n">
         <v>27.25</v>
@@ -5320,7 +5320,7 @@
         <v>1</v>
       </c>
       <c r="L60" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60" s="6" t="n">
         <v>32.88</v>
@@ -5401,7 +5401,7 @@
         <v>1</v>
       </c>
       <c r="L61" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61" s="6" t="n">
         <v>81.38</v>
@@ -5482,7 +5482,7 @@
         <v>1</v>
       </c>
       <c r="L62" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M62" s="6" t="n">
         <v>7.15</v>
@@ -5563,7 +5563,7 @@
         <v>1</v>
       </c>
       <c r="L63" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M63" s="6" t="n">
         <v>4.65</v>
@@ -5644,7 +5644,7 @@
         <v>1</v>
       </c>
       <c r="L64" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M64" s="6" t="n">
         <v>37.38</v>
@@ -5725,7 +5725,7 @@
         <v>1</v>
       </c>
       <c r="L65" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M65" s="6" t="n">
         <v>31.8</v>
@@ -5806,7 +5806,7 @@
         <v>1</v>
       </c>
       <c r="L66" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M66" s="6" t="n">
         <v>14.5</v>
@@ -5887,7 +5887,7 @@
         <v>1</v>
       </c>
       <c r="L67" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M67" s="6" t="n">
         <v>17</v>
@@ -5968,7 +5968,7 @@
         <v>3</v>
       </c>
       <c r="L68" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M68" s="6" t="n">
         <v>113.05</v>
@@ -6135,7 +6135,7 @@
         </is>
       </c>
       <c r="C82" s="5" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>